<commit_message>
separate submitting and non submitting files
</commit_message>
<xml_diff>
--- a/formated_data.xlsx
+++ b/formated_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penghaochen/Dropbox/Master/2021_22 SEM1/FE5209/Project/covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B634010C-6C4B-2745-82D3-649E4669CF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBACDF6-719A-2544-B54F-3AD344D36E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily New Cases" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="75">
   <si>
     <t>Singapore</t>
   </si>
@@ -257,13 +257,26 @@
   <si>
     <t>MUR</t>
   </si>
+  <si>
+    <t>2021-06</t>
+  </si>
+  <si>
+    <t>2021-07</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -378,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,6 +431,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32337,7 +32355,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
@@ -32353,7 +32371,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
@@ -32363,7 +32381,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4">
@@ -32373,7 +32391,7 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
@@ -32383,7 +32401,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4">
@@ -32393,7 +32411,7 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4">
@@ -32403,7 +32421,7 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4">
@@ -32413,7 +32431,7 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4">
@@ -32423,7 +32441,7 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4">
@@ -32433,7 +32451,7 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4">
@@ -32443,7 +32461,7 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4">
@@ -32453,7 +32471,7 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4">
@@ -32463,7 +32481,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4">
@@ -32473,7 +32491,7 @@
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4">
@@ -32483,7 +32501,7 @@
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4">
@@ -32493,7 +32511,7 @@
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="4">
@@ -32503,7 +32521,7 @@
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="4">
@@ -32513,7 +32531,7 @@
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="16" thickBot="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="4">
@@ -32556,7 +32574,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B50"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32570,7 +32588,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="18">
@@ -32578,7 +32596,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="18">
@@ -32586,7 +32604,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="18">
@@ -32594,7 +32612,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="18">
@@ -32602,7 +32620,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="18">
@@ -32610,7 +32628,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="18">
@@ -32618,7 +32636,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="18">
@@ -32626,7 +32644,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="18">
@@ -32634,7 +32652,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="18">
@@ -32642,7 +32660,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="18">
@@ -32650,7 +32668,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="18">
@@ -32658,7 +32676,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="18">
@@ -32666,7 +32684,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="18">
@@ -32674,7 +32692,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="18">
@@ -32682,7 +32700,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="18">
@@ -32690,7 +32708,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="18">
@@ -32698,7 +32716,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="18">
@@ -32706,7 +32724,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="18">
@@ -32714,7 +32732,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="18">
@@ -32722,7 +32740,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="18">
@@ -32730,7 +32748,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="18">
@@ -32738,7 +32756,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="18">
@@ -32746,7 +32764,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="18">
@@ -32754,7 +32772,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="18">
@@ -32762,7 +32780,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="18">
@@ -32770,7 +32788,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="18">
@@ -32778,7 +32796,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="18">
@@ -32786,7 +32804,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="18">
@@ -32794,7 +32812,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="18">
@@ -32802,7 +32820,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="18">
@@ -32810,7 +32828,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="18">
@@ -32818,7 +32836,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="18">
@@ -32826,7 +32844,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="18">
@@ -32834,7 +32852,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="18">
@@ -32842,7 +32860,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="18">
@@ -32850,7 +32868,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="18">
@@ -32858,7 +32876,7 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="18">
@@ -32866,7 +32884,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B39" s="18">
@@ -32874,7 +32892,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B40" s="18">
@@ -32882,7 +32900,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="18">
@@ -32890,7 +32908,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B42" s="18">
@@ -32898,7 +32916,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B43" s="18">
@@ -32906,7 +32924,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B44" s="18">
@@ -32914,7 +32932,7 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="18">
@@ -32922,7 +32940,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="18">
@@ -32930,7 +32948,7 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="18">
@@ -32938,7 +32956,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="18">
@@ -32946,7 +32964,7 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="18">
@@ -32954,7 +32972,7 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="20" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="18">
@@ -32970,8 +32988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA443B4-1472-2D45-9244-C57EC4F8EB60}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A50" sqref="A47:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32985,7 +33003,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="18">
@@ -32993,7 +33011,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="18">
@@ -33001,7 +33019,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="18">
@@ -33009,7 +33027,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="18">
@@ -33017,7 +33035,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="18">
@@ -33025,7 +33043,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="18">
@@ -33033,7 +33051,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="18">
@@ -33041,7 +33059,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="18">
@@ -33049,7 +33067,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="18">
@@ -33057,7 +33075,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="18">
@@ -33065,7 +33083,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="18">
@@ -33073,7 +33091,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="18">
@@ -33081,7 +33099,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="18">
@@ -33089,7 +33107,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="18">
@@ -33097,7 +33115,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="18">
@@ -33105,7 +33123,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="18">
@@ -33113,7 +33131,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="18">
@@ -33121,7 +33139,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="18">
@@ -33129,7 +33147,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="18">
@@ -33137,7 +33155,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="18">
@@ -33145,7 +33163,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="18">
@@ -33153,7 +33171,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="19" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="18">
@@ -33161,7 +33179,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="18">
@@ -33169,7 +33187,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="19" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="18">
@@ -33177,7 +33195,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="18">
@@ -33185,7 +33203,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="18">
@@ -33193,7 +33211,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="18">
@@ -33201,7 +33219,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="18">
@@ -33209,7 +33227,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="18">
@@ -33217,7 +33235,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="18">
@@ -33225,7 +33243,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="18">
@@ -33233,7 +33251,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="18">
@@ -33241,7 +33259,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="18">
@@ -33249,7 +33267,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="18">
@@ -33257,7 +33275,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="19" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="18">
@@ -33265,7 +33283,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="18">
@@ -33273,7 +33291,7 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="19" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="18">
@@ -33281,7 +33299,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B39" s="18">
@@ -33289,7 +33307,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B40" s="18">
@@ -33297,7 +33315,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="18">
@@ -33305,7 +33323,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B42" s="18">
@@ -33313,7 +33331,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B43" s="18">
@@ -33321,7 +33339,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B44" s="18">
@@ -33329,7 +33347,7 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="18">
@@ -33337,7 +33355,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="18">
@@ -33345,7 +33363,7 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="18">
@@ -33353,7 +33371,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="18">
@@ -33361,7 +33379,7 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="19" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="18">
@@ -33369,7 +33387,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" thickBot="1">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="18">
@@ -33401,8 +33419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D070761-CC06-BB48-B07B-7D97B3F06019}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -33422,8 +33440,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="11">
-        <v>44348</v>
+      <c r="A2" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="B2" s="10">
         <v>2.7</v>
@@ -33436,8 +33454,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1">
-      <c r="A3" s="11">
-        <v>44378</v>
+      <c r="A3" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="B3" s="10">
         <v>2.8</v>
@@ -33450,8 +33468,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1">
-      <c r="A4" s="11">
-        <v>44409</v>
+      <c r="A4" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="10">
         <v>2.7</v>
@@ -33464,8 +33482,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1">
-      <c r="A5" s="11">
-        <v>44440</v>
+      <c r="A5" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="B5" s="10">
         <v>2.6</v>

</xml_diff>

<commit_message>
refine the unemployment prediction script
</commit_message>
<xml_diff>
--- a/formated_data.xlsx
+++ b/formated_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penghaochen/Dropbox/Master/2021_22 SEM1/FE5209/Project/covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBACDF6-719A-2544-B54F-3AD344D36E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE8DDF4-B645-BF47-A014-D2A729CD4782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily New Cases" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="m/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -312,6 +312,12 @@
       <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF494444"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -391,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -436,6 +442,7 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32571,10 +32578,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54AE73C-BF2E-6F47-A614-7EC13866BAA4}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:BF50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -32591,392 +32598,445 @@
       <c r="A2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="18">
-        <v>4.4254020000000001</v>
+      <c r="B2">
+        <v>4.43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="18">
-        <v>4.3376950000000001</v>
+      <c r="B3">
+        <v>4.34</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="18">
-        <v>4.3280399999999997</v>
+      <c r="B4">
+        <v>4.33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="18">
-        <v>4.2668150000000002</v>
+      <c r="B5">
+        <v>4.2699999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="18">
-        <v>4.2433370000000004</v>
+      <c r="B6">
+        <v>4.24</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="18">
-        <v>4.2718559999999997</v>
+      <c r="B7">
+        <v>4.2699999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="18">
-        <v>4.3522169999999996</v>
+      <c r="B8">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="18">
-        <v>4.3060479999999997</v>
+      <c r="B9">
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="18">
-        <v>4.2130970000000003</v>
+      <c r="B10">
+        <v>4.21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="18">
-        <v>4.198035</v>
+      <c r="B11">
+        <v>4.2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="18">
-        <v>4.1889440000000002</v>
+      <c r="B12">
+        <v>4.1900000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="18">
-        <v>4.1653599999999997</v>
+      <c r="B13">
+        <v>4.17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="18">
-        <v>4.036543</v>
+      <c r="B14">
+        <v>4.04</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="18">
-        <v>4.0211969999999999</v>
+      <c r="B15">
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="18">
-        <v>4.0346690000000001</v>
+      <c r="B16">
+        <v>4.03</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18">
-        <v>4.0733689999999996</v>
+      <c r="B17">
+        <v>4.07</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="18">
-        <v>4.0553179999999998</v>
+      <c r="B18">
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="18">
-        <v>4.0390870000000003</v>
+      <c r="B19">
+        <v>4.04</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="18">
-        <v>4.0135420000000002</v>
+      <c r="B20">
+        <v>4.01</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="18">
-        <v>3.9305620000000001</v>
+      <c r="B21">
+        <v>3.93</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="18">
-        <v>3.9415309999999999</v>
+      <c r="B22">
+        <v>3.94</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="18">
-        <v>3.8178010000000002</v>
+      <c r="B23">
+        <v>3.82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="18">
-        <v>3.8302740000000002</v>
+      <c r="B24">
+        <v>3.83</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="18">
-        <v>3.7956110000000001</v>
+      <c r="B25">
+        <v>3.8</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="18">
-        <v>3.8928379999999998</v>
+      <c r="B26">
+        <v>3.89</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="18">
-        <v>3.7970489999999999</v>
+      <c r="B27">
+        <v>3.8</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="18">
-        <v>3.8627410000000002</v>
+      <c r="B28">
+        <v>3.86</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="18">
-        <v>3.8331979999999999</v>
+      <c r="B29">
+        <v>3.83</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="18">
-        <v>3.7571340000000002</v>
+      <c r="B30">
+        <v>3.76</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="18">
-        <v>3.8185630000000002</v>
+      <c r="B31">
+        <v>3.82</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="18">
-        <v>3.768513</v>
+      <c r="B32">
+        <v>3.77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="18">
-        <v>3.912849</v>
+      <c r="B33">
+        <v>3.91</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="18">
-        <v>3.9612129999999999</v>
+      <c r="B34">
+        <v>3.96</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="18">
-        <v>3.996721</v>
+      <c r="B35">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="18">
-        <v>4.0413800000000002</v>
+      <c r="B36">
+        <v>4.04</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="18">
-        <v>4.1469899999999997</v>
+      <c r="B37">
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="18">
-        <v>4.1371890000000002</v>
+      <c r="B38">
+        <v>4.1399999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="18">
-        <v>4.3189039999999999</v>
+      <c r="B39">
+        <v>4.32</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="18">
-        <v>4.5383909999999998</v>
+      <c r="B40">
+        <v>4.54</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="18">
-        <v>4.8480699999999999</v>
+      <c r="B41">
+        <v>4.8499999999999996</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="18">
-        <v>5.0499239999999999</v>
+      <c r="B42">
+        <v>5.05</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="18">
-        <v>5.1072100000000002</v>
+      <c r="B43">
+        <v>5.1100000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="18">
-        <v>5.2198320000000002</v>
+      <c r="B44">
+        <v>5.22</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="18">
-        <v>5.1340260000000004</v>
+      <c r="B45">
+        <v>5.13</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="18">
-        <v>5.034872</v>
+      <c r="B46">
+        <v>5.03</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="18">
-        <v>4.8856159999999997</v>
+      <c r="B47">
+        <v>4.8899999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="18">
-        <v>4.8407559999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="B48">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:58" ht="18">
       <c r="A49" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="18">
-        <v>4.8394430000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="B49">
+        <v>4.84</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+      <c r="V49" s="22"/>
+      <c r="W49" s="22"/>
+      <c r="X49" s="22"/>
+      <c r="Y49" s="22"/>
+      <c r="Z49" s="22"/>
+      <c r="AA49" s="22"/>
+      <c r="AB49" s="22"/>
+      <c r="AC49" s="22"/>
+      <c r="AD49" s="22"/>
+      <c r="AE49" s="22"/>
+      <c r="AF49" s="22"/>
+      <c r="AG49" s="22"/>
+      <c r="AH49" s="22"/>
+      <c r="AI49" s="22"/>
+      <c r="AJ49" s="22"/>
+      <c r="AK49" s="22"/>
+      <c r="AL49" s="22"/>
+      <c r="AM49" s="22"/>
+      <c r="AN49" s="22"/>
+      <c r="AO49" s="22"/>
+      <c r="AP49" s="22"/>
+      <c r="AQ49" s="22"/>
+      <c r="AR49" s="22"/>
+      <c r="AS49" s="22"/>
+      <c r="AT49" s="22"/>
+      <c r="AU49" s="22"/>
+      <c r="AV49" s="22"/>
+      <c r="AW49" s="22"/>
+      <c r="AX49" s="22"/>
+      <c r="AY49" s="22"/>
+      <c r="AZ49" s="22"/>
+      <c r="BA49" s="22"/>
+      <c r="BB49" s="22"/>
+      <c r="BC49" s="22"/>
+      <c r="BD49" s="22"/>
+      <c r="BE49" s="22"/>
+      <c r="BF49" s="22"/>
+    </row>
+    <row r="50" spans="1:58">
       <c r="A50" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="18">
-        <v>4.7239149999999999</v>
+      <c r="B50">
+        <v>4.72</v>
       </c>
     </row>
   </sheetData>
@@ -33419,8 +33479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D070761-CC06-BB48-B07B-7D97B3F06019}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>